<commit_message>
Added License, Added routing, Added submitted page
</commit_message>
<xml_diff>
--- a/demo_documents/DemoExcel.xlsx
+++ b/demo_documents/DemoExcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="g:\docusign project\quickstart app-1-node.js\demo_documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B0FC452-2037-48FB-9394-B53D4E10D144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF6A9ADE-40B4-4E90-9550-011898CD4AE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32265" yWindow="3465" windowWidth="21600" windowHeight="11385" xr2:uid="{003732AD-2884-4E55-A70A-C533FE2671B4}"/>
+    <workbookView xWindow="7425" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{003732AD-2884-4E55-A70A-C533FE2671B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>name</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>signer</t>
+  </si>
+  <si>
+    <t>340813412@yrdsb.ca</t>
   </si>
 </sst>
 </file>
@@ -434,13 +437,13 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" customWidth="1"/>
     <col min="3" max="3" width="35.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -478,12 +481,21 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="1"/>
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{E2B77774-CE06-4317-9DC9-8620B616C4B5}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{773D5884-7FFA-484D-8FCB-169B3E219583}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{29550AB5-C884-4298-ACA8-25518E136719}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>